<commit_message>
Inserte reference in tag
</commit_message>
<xml_diff>
--- a/EVENTURI/eventuri_code/eventuri_all_stars_import_catalogue_new.xlsx
+++ b/EVENTURI/eventuri_code/eventuri_all_stars_import_catalogue_new.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Global - Sep-19-2023" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Global - Sep-22-2023" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Price List" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="GBP" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="EUR" sheetId="4" state="hidden" r:id="rId4"/>
@@ -1937,7 +1937,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>manufacturer</t>
+          <t>Manufacturer</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1992,7 +1992,7 @@
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>Product</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
@@ -2087,12 +2087,12 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Audi,S1,2.0,TFSI,Black,Carbon,intake</t>
+          <t>Audi S1 2.0 TFSI Black Carbon intake</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Audi,S1,2.0,TFSI,Black,Carbon,intake</t>
+          <t>Audi S1 2.0 TFSI Black Carbon intake</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -2162,12 +2162,12 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Audi,S3,8Y,2020+,,TTS,2022+,Carbon,Intake</t>
+          <t>Audi S3 8Y 2020+, TTS 2022+ Carbon Intake</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Audi,S3,8Y,2020+,,TTS,2022+,Carbon,Intake</t>
+          <t>Audi S3 8Y 2020+, TTS 2022+ Carbon Intake</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -2239,12 +2239,12 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Audi,S3,8V,2.0,TFSI,Full,Black,Carbon,intake</t>
+          <t>Audi S3 8V 2.0 TFSI Full Black Carbon intake</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Audi,S3,8V,2.0,TFSI,Full,Black,Carbon,intake</t>
+          <t>Audi S3 8V 2.0 TFSI Full Black Carbon intake</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -2314,12 +2314,12 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Audi,8V,RS3,LHD,Full,Black,Carbon,intake,Gen,1</t>
+          <t>Audi 8V RS3 LHD Full Black Carbon intake Gen 1</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Audi,8V,RS3,LHD,Full,Black,Carbon,intake,Gen,1</t>
+          <t>Audi 8V RS3 LHD Full Black Carbon intake Gen 1</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -2389,12 +2389,12 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Audi,8V,RS3,RHD,Full,Black,Carbon,intake,Gen,1</t>
+          <t>Audi 8V RS3 RHD Full Black Carbon intake Gen 1</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Audi,8V,RS3,RHD,Full,Black,Carbon,intake,Gen,1</t>
+          <t>Audi 8V RS3 RHD Full Black Carbon intake Gen 1</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -2466,12 +2466,12 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Audi,RS3,Gen,2,/,TTRS,8S,intake,for,DAZA,and,DWNA,Engines</t>
+          <t>Audi RS3 Gen 2 / TTRS 8S intake for DAZA and DWNA Engines</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Audi,RS3,Gen,2,/,TTRS,8S,intake,for,DAZA,and,DWNA,Engines</t>
+          <t>Audi RS3 Gen 2 / TTRS 8S intake for DAZA and DWNA Engines</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -2545,12 +2545,12 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Audi,RS3,Gen,2,Duct,for,APR,Throttle,Body</t>
+          <t>Audi RS3 Gen 2 Duct for APR Throttle Body</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Audi,RS3,Gen,2,Duct,for,APR,Throttle,Body</t>
+          <t>Audi RS3 Gen 2 Duct for APR Throttle Body</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -2620,12 +2620,12 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Audi,RS3,Carbon,Headlamp,Race,Ducts,for,Stage,3,intake</t>
+          <t>Audi RS3 Carbon Headlamp Race Ducts for Stage 3 intake</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Audi,RS3,Carbon,Headlamp,Race,Ducts,for,Stage,3,intake</t>
+          <t>Audi RS3 Carbon Headlamp Race Ducts for Stage 3 intake</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -2697,12 +2697,12 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Audi,RS3,8Y,2020+,Carbon,Intake</t>
+          <t>Audi RS3 8Y 2020+ Carbon Intake</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Audi,RS3,8Y,2020+,Carbon,Intake</t>
+          <t>Audi RS3 8Y 2020+ Carbon Intake</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -2774,12 +2774,12 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Audi,RS3,/,TTRS,Gen,2,8V,8Y,LHD,Carbon,turbo,inlet,with,NO,FLANGE</t>
+          <t>Audi RS3 / TTRS Gen 2 8V 8Y LHD Carbon turbo inlet with NO FLANGE</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Audi,RS3,/,TTRS,Gen,2,8V,8Y,LHD,Carbon,turbo,inlet,with,NO,FLANGE</t>
+          <t>Audi RS3 / TTRS Gen 2 8V 8Y LHD Carbon turbo inlet with NO FLANGE</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -2851,12 +2851,12 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Audi,RS3,/,TTRS,Gen,2,8V,8Y,RHD,Carbon,turbo,inlet,with,NO,FLANGE</t>
+          <t>Audi RS3 / TTRS Gen 2 8V 8Y RHD Carbon turbo inlet with NO FLANGE</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Audi,RS3,/,TTRS,Gen,2,8V,8Y,RHD,Carbon,turbo,inlet,with,NO,FLANGE</t>
+          <t>Audi RS3 / TTRS Gen 2 8V 8Y RHD Carbon turbo inlet with NO FLANGE</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -2926,12 +2926,12 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Stock,Turbo,Flange,for,RS3/TTRS,Carbon,Turbo,Inlet</t>
+          <t>Stock Turbo Flange for RS3/TTRS Carbon Turbo Inlet</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Stock,Turbo,Flange,for,RS3/TTRS,Carbon,Turbo,Inlet</t>
+          <t>Stock Turbo Flange for RS3/TTRS Carbon Turbo Inlet</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -3001,12 +3001,12 @@
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>TTE700/625,Turbo,Flange,for,RS3/TTRS,Carbon,Turbo,Inlet</t>
+          <t>TTE700/625 Turbo Flange for RS3/TTRS Carbon Turbo Inlet</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>TTE700/625,Turbo,Flange,for,RS3/TTRS,Carbon,Turbo,Inlet</t>
+          <t>TTE700/625 Turbo Flange for RS3/TTRS Carbon Turbo Inlet</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -3076,12 +3076,12 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>SRM,GTX,Turbo,Flange,for,RS3/TTRS,Carbon,Turbo,Inlet</t>
+          <t>SRM GTX Turbo Flange for RS3/TTRS Carbon Turbo Inlet</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>SRM,GTX,Turbo,Flange,for,RS3/TTRS,Carbon,Turbo,Inlet</t>
+          <t>SRM GTX Turbo Flange for RS3/TTRS Carbon Turbo Inlet</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -3153,12 +3153,12 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Audi,RS3,Gen,2,/,TTRS,8S,Black,and,Red,Engine,Cover</t>
+          <t>Audi RS3 Gen 2 / TTRS 8S Black and Red Engine Cover</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Audi,RS3,Gen,2,/,TTRS,8S,Black,and,Red,Engine,Cover</t>
+          <t>Audi RS3 Gen 2 / TTRS 8S Black and Red Engine Cover</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -3230,12 +3230,12 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Audi,RSQ3,F3,2019+,Carbon,Intake</t>
+          <t>Audi RSQ3 F3 2019+ Carbon Intake</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Audi,RSQ3,F3,2019+,Carbon,Intake</t>
+          <t>Audi RSQ3 F3 2019+ Carbon Intake</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -3307,12 +3307,12 @@
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Audi,RSQ3,DWNA,Adapter,set</t>
+          <t>Audi RSQ3 DWNA Adapter set</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>Audi,RSQ3,DWNA,Adapter,set</t>
+          <t>Audi RSQ3 DWNA Adapter set</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -3384,12 +3384,12 @@
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Audi,B8,RS5/RS4,Black,Carbon,intake</t>
+          <t>Audi B8 RS5/RS4 Black Carbon intake</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>Audi,B8,RS5/RS4,Black,Carbon,intake</t>
+          <t>Audi B8 RS5/RS4 Black Carbon intake</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -3459,12 +3459,12 @@
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Audi,B8,RS4,Black,Carbon,Slam,Panel,Cover</t>
+          <t>Audi B8 RS4 Black Carbon Slam Panel Cover</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>Audi,B8,RS4,Black,Carbon,Slam,Panel,Cover</t>
+          <t>Audi B8 RS4 Black Carbon Slam Panel Cover</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -3534,12 +3534,12 @@
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Audi,B8,RS5,Black,Carbon,Facelift,Slam,Panel,Cover</t>
+          <t>Audi B8 RS5 Black Carbon Facelift Slam Panel Cover</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>Audi,B8,RS5,Black,Carbon,Facelift,Slam,Panel,Cover</t>
+          <t>Audi B8 RS5 Black Carbon Facelift Slam Panel Cover</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -3609,12 +3609,12 @@
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Audi,B8,RS5/RS4,Black,Carbon,Engine,Cover</t>
+          <t>Audi B8 RS5/RS4 Black Carbon Engine Cover</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>Audi,B8,RS5/RS4,Black,Carbon,Engine,Cover</t>
+          <t>Audi B8 RS5/RS4 Black Carbon Engine Cover</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -3684,12 +3684,12 @@
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Audi,B9,S5/S4,Black,Carbon,intake</t>
+          <t>Audi B9 S5/S4 Black Carbon intake</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>Audi,B9,S5/S4,Black,Carbon,intake</t>
+          <t>Audi B9 S5/S4 Black Carbon intake</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -3761,12 +3761,12 @@
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Audi,B9,RS5/RS4,Black,Carbon,intake,with,secondary,duct</t>
+          <t>Audi B9 RS5/RS4 Black Carbon intake with secondary duct</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>Audi,B9,RS5/RS4,Black,Carbon,intake,with,secondary,duct</t>
+          <t>Audi B9 RS5/RS4 Black Carbon intake with secondary duct</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -3836,12 +3836,12 @@
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Audi,C7,S6,S7,Black,Carbon,intake</t>
+          <t>Audi C7 S6 S7 Black Carbon intake</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>Audi,C7,S6,S7,Black,Carbon,intake</t>
+          <t>Audi C7 S6 S7 Black Carbon intake</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -3911,12 +3911,12 @@
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Audi,SQ7,/,SQ8,2020+,4.0,TFSI,V8,Twin,Turbo,Intake</t>
+          <t>Audi SQ7 / SQ8 2020+ 4.0 TFSI V8 Twin Turbo Intake</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>Audi,SQ7,/,SQ8,2020+,4.0,TFSI,V8,Twin,Turbo,Intake</t>
+          <t>Audi SQ7 / SQ8 2020+ 4.0 TFSI V8 Twin Turbo Intake</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -3986,12 +3986,12 @@
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Audi,C7,RS6,RS7,Black,Carbon,intake</t>
+          <t>Audi C7 RS6 RS7 Black Carbon intake</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>Audi,C7,RS6,RS7,Black,Carbon,intake</t>
+          <t>Audi C7 RS6 RS7 Black Carbon intake</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -4061,12 +4061,12 @@
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Audi,C8,RS6,RS7,Black,Carbon,intake,Gloss</t>
+          <t>Audi C8 RS6 RS7 Black Carbon intake Gloss</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>Audi,C8,RS6,RS7,Black,Carbon,intake,Gloss</t>
+          <t>Audi C8 RS6 RS7 Black Carbon intake Gloss</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -4136,12 +4136,12 @@
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Audi,C8,RS6,RS7,Black,Carbon,intake,Matte</t>
+          <t>Audi C8 RS6 RS7 Black Carbon intake Matte</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>Audi,C8,RS6,RS7,Black,Carbon,intake,Matte</t>
+          <t>Audi C8 RS6 RS7 Black Carbon intake Matte</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -4211,12 +4211,12 @@
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Audi,C8,RS6,RS7,TTE,888/1020,Hybrid,Turbo,Inlets,</t>
+          <t xml:space="preserve">Audi C8 RS6 RS7 TTE 888/1020 Hybrid Turbo Inlets </t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>Audi,C8,RS6,RS7,TTE,888/1020,Hybrid,Turbo,Inlets,</t>
+          <t xml:space="preserve">Audi C8 RS6 RS7 TTE 888/1020 Hybrid Turbo Inlets </t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -4286,12 +4286,12 @@
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Audi,C8,RS6,RS7,Black,Carbon,Engine,Cover,Gloss</t>
+          <t>Audi C8 RS6 RS7 Black Carbon Engine Cover Gloss</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>Audi,C8,RS6,RS7,Black,Carbon,Engine,Cover,Gloss</t>
+          <t>Audi C8 RS6 RS7 Black Carbon Engine Cover Gloss</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -4361,12 +4361,12 @@
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Audi,C8,RS6,RS7,Black,Carbon,Engine,Cover,Matte</t>
+          <t>Audi C8 RS6 RS7 Black Carbon Engine Cover Matte</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>Audi,C8,RS6,RS7,Black,Carbon,Engine,Cover,Matte</t>
+          <t>Audi C8 RS6 RS7 Black Carbon Engine Cover Matte</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -4436,12 +4436,12 @@
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Audi,C8,RS6,2023,Breather,Adapter,Kit</t>
+          <t>Audi C8 RS6 2023 Breather Adapter Kit</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>Audi,C8,RS6,2023,Breather,Adapter,Kit</t>
+          <t>Audi C8 RS6 2023 Breather Adapter Kit</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -4511,12 +4511,12 @@
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Audi,RSQ7,/,RSQ8,2020+,4.0,TFSI,V8,Twin,Turbo,Intake</t>
+          <t>Audi RSQ7 / RSQ8 2020+ 4.0 TFSI V8 Twin Turbo Intake</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>Audi,RSQ7,/,RSQ8,2020+,4.0,TFSI,V8,Twin,Turbo,Intake</t>
+          <t>Audi RSQ7 / RSQ8 2020+ 4.0 TFSI V8 Twin Turbo Intake</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -4586,12 +4586,12 @@
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Audi,R8,V10,4S,2015+</t>
+          <t>Audi R8 V10 4S 2015+</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>Audi,R8,V10,4S,2015+</t>
+          <t>Audi R8 V10 4S 2015+</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -4661,12 +4661,12 @@
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Bentayga,4.0,TFSI,V8,Twin,Turbo,Intake,</t>
+          <t xml:space="preserve">Bentayga 4.0 TFSI V8 Twin Turbo Intake </t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>Bentayga,4.0,TFSI,V8,Twin,Turbo,Intake,</t>
+          <t xml:space="preserve">Bentayga 4.0 TFSI V8 Twin Turbo Intake </t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -4736,12 +4736,12 @@
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>BMW,B58,M140i,,M240i,,M340i,Black,Carbon,intake</t>
+          <t>BMW B58 M140i, M240i, M340i Black Carbon intake</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>BMW,B58,M140i,,M240i,,M340i,Black,Carbon,intake</t>
+          <t>BMW B58 M140i, M240i, M340i Black Carbon intake</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -4811,12 +4811,12 @@
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>BMW,B58,M140i,,M240i,,M340i,,F,Series,Carbon,Engine,Cover</t>
+          <t>BMW B58 M140i, M240i, M340i  F Series Carbon Engine Cover</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>BMW,B58,M140i,,M240i,,M340i,,F,Series,Carbon,Engine,Cover</t>
+          <t>BMW B58 M140i, M240i, M340i  F Series Carbon Engine Cover</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
@@ -4886,12 +4886,12 @@
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>BMW,E39,M5,Black,Carbon,intake</t>
+          <t>BMW E39 M5 Black Carbon intake</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>BMW,E39,M5,Black,Carbon,intake</t>
+          <t>BMW E39 M5 Black Carbon intake</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
@@ -4961,12 +4961,12 @@
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>BMW,E46,M3,Black,Carbon,intake</t>
+          <t>BMW E46 M3 Black Carbon intake</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>BMW,E46,M3,Black,Carbon,intake</t>
+          <t>BMW E46 M3 Black Carbon intake</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
@@ -5036,12 +5036,12 @@
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>BMW,E46,M3,Carbon,Scoop,</t>
+          <t xml:space="preserve">BMW E46 M3 Carbon Scoop </t>
         </is>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>BMW,E46,M3,Carbon,Scoop,</t>
+          <t xml:space="preserve">BMW E46 M3 Carbon Scoop </t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
@@ -5111,12 +5111,12 @@
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>BMW,E6X,M5/M6,Black,Carbon,intake</t>
+          <t>BMW E6X M5/M6 Black Carbon intake</t>
         </is>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>BMW,E6X,M5/M6,Black,Carbon,intake</t>
+          <t>BMW E6X M5/M6 Black Carbon intake</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
@@ -5188,12 +5188,12 @@
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>BMW,E9X,M3,Black,Carbon,intake,Gloss</t>
+          <t>BMW E9X M3 Black Carbon intake Gloss</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>BMW,E9X,M3,Black,Carbon,intake,Gloss</t>
+          <t>BMW E9X M3 Black Carbon intake Gloss</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
@@ -5265,12 +5265,12 @@
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>BMW,E9X,M3,Black,Carbon,intake,Matte</t>
+          <t>BMW E9X M3 Black Carbon intake Matte</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>BMW,E9X,M3,Black,Carbon,intake,Matte</t>
+          <t>BMW E9X M3 Black Carbon intake Matte</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
@@ -5340,12 +5340,12 @@
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>BMW,E9X,M3,Carbon,Inlet,Plenum,Gloss</t>
+          <t>BMW E9X M3 Carbon Inlet Plenum Gloss</t>
         </is>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>BMW,E9X,M3,Carbon,Inlet,Plenum,Gloss</t>
+          <t>BMW E9X M3 Carbon Inlet Plenum Gloss</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
@@ -5415,12 +5415,12 @@
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>BMW,E9X,M3,Carbon,Inlet,Plenum,Matte</t>
+          <t>BMW E9X M3 Carbon Inlet Plenum Matte</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>BMW,E9X,M3,Carbon,Inlet,Plenum,Matte</t>
+          <t>BMW E9X M3 Carbon Inlet Plenum Matte</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
@@ -5492,12 +5492,12 @@
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>BMW,E9X,M3,Carbon,Airbox,Lid,Gloss</t>
+          <t>BMW E9X M3 Carbon Airbox Lid Gloss</t>
         </is>
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>BMW,E9X,M3,Carbon,Airbox,Lid,Gloss</t>
+          <t>BMW E9X M3 Carbon Airbox Lid Gloss</t>
         </is>
       </c>
       <c r="R47" t="inlineStr">
@@ -5569,12 +5569,12 @@
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>BMW,E9X,M3,Carbon,Airbox,Lid,Matte</t>
+          <t>BMW E9X M3 Carbon Airbox Lid Matte</t>
         </is>
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>BMW,E9X,M3,Carbon,Airbox,Lid,Matte</t>
+          <t>BMW E9X M3 Carbon Airbox Lid Matte</t>
         </is>
       </c>
       <c r="R48" t="inlineStr">
@@ -5644,12 +5644,12 @@
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>BMW,E9X,M3,Carbon,Duct,Set,Gloss</t>
+          <t>BMW E9X M3 Carbon Duct Set Gloss</t>
         </is>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>BMW,E9X,M3,Carbon,Duct,Set,Gloss</t>
+          <t>BMW E9X M3 Carbon Duct Set Gloss</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
@@ -5719,12 +5719,12 @@
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>BMW,E9X,M3,Carbon,Duct,Set,Matte</t>
+          <t>BMW E9X M3 Carbon Duct Set Matte</t>
         </is>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>BMW,E9X,M3,Carbon,Duct,Set,Matte</t>
+          <t>BMW E9X M3 Carbon Duct Set Matte</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
@@ -5794,12 +5794,12 @@
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>BMW,S55,Carbon,Chargepipes,-,Set,of,2,Upper,Chargepipes</t>
+          <t>BMW S55 Carbon Chargepipes - Set of 2 Upper Chargepipes</t>
         </is>
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>BMW,S55,Carbon,Chargepipes,-,Set,of,2,Upper,Chargepipes</t>
+          <t>BMW S55 Carbon Chargepipes - Set of 2 Upper Chargepipes</t>
         </is>
       </c>
       <c r="R51" t="inlineStr">
@@ -5869,12 +5869,12 @@
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>BMW,S62,V8,Carbon,Plenum,Lid,for,E39,M5,and,Z8</t>
+          <t>BMW S62 V8 Carbon Plenum Lid for E39 M5 and Z8</t>
         </is>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>BMW,S62,V8,Carbon,Plenum,Lid,for,E39,M5,and,Z8</t>
+          <t>BMW S62 V8 Carbon Plenum Lid for E39 M5 and Z8</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
@@ -5944,12 +5944,12 @@
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>BMW,F8X,M3/M4,V2,Full,Black,Carbon,intake,with,SEALED,Carbon,ducts</t>
+          <t>BMW F8X M3/M4 V2 Full Black Carbon intake with SEALED Carbon ducts</t>
         </is>
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>BMW,F8X,M3/M4,V2,Full,Black,Carbon,intake,with,SEALED,Carbon,ducts</t>
+          <t>BMW F8X M3/M4 V2 Full Black Carbon intake with SEALED Carbon ducts</t>
         </is>
       </c>
       <c r="R53" t="inlineStr">
@@ -6019,12 +6019,12 @@
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>BMW,F8X,M3/M4,Black,Carbon,Seat,Back,Covers</t>
+          <t>BMW F8X M3/M4 Black Carbon Seat Back Covers</t>
         </is>
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>BMW,F8X,M3/M4,Black,Carbon,Seat,Back,Covers</t>
+          <t>BMW F8X M3/M4 Black Carbon Seat Back Covers</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
@@ -6096,12 +6096,12 @@
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>BMW,F8X,M3/M4,Black,Carbon,,Engine,Cover</t>
+          <t>BMW F8X M3/M4 Black Carbon  Engine Cover</t>
         </is>
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>BMW,F8X,M3/M4,Black,Carbon,,Engine,Cover</t>
+          <t>BMW F8X M3/M4 Black Carbon  Engine Cover</t>
         </is>
       </c>
       <c r="R55" t="inlineStr">
@@ -6171,12 +6171,12 @@
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>BMW,F9X,M5/M8,Black,Carbon,intake,with,shrouds</t>
+          <t>BMW F9X M5/M8 Black Carbon intake with shrouds</t>
         </is>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>BMW,F9X,M5/M8,Black,Carbon,intake,with,shrouds</t>
+          <t>BMW F9X M5/M8 Black Carbon intake with shrouds</t>
         </is>
       </c>
       <c r="R56" t="inlineStr">
@@ -6248,12 +6248,12 @@
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>BMW,F9X,M5,Shroud,set,for,upgrading,V1,intake</t>
+          <t>BMW F9X M5 Shroud set for upgrading V1 intake</t>
         </is>
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>BMW,F9X,M5,Shroud,set,for,upgrading,V1,intake</t>
+          <t>BMW F9X M5 Shroud set for upgrading V1 intake</t>
         </is>
       </c>
       <c r="R57" t="inlineStr">
@@ -6323,12 +6323,12 @@
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>BMW,F9X,M5/M8,Turbo,Inlets</t>
+          <t>BMW F9X M5/M8 Turbo Inlets</t>
         </is>
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>BMW,F9X,M5/M8,Turbo,Inlets</t>
+          <t>BMW F9X M5/M8 Turbo Inlets</t>
         </is>
       </c>
       <c r="R58" t="inlineStr">
@@ -6398,12 +6398,12 @@
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>BMW,F10,M5,Full,Black,Carbon,intake</t>
+          <t>BMW F10 M5 Full Black Carbon intake</t>
         </is>
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>BMW,F10,M5,Full,Black,Carbon,intake</t>
+          <t>BMW F10 M5 Full Black Carbon intake</t>
         </is>
       </c>
       <c r="R59" t="inlineStr">
@@ -6473,12 +6473,12 @@
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>BMW,F1X,M6,Full,Black,Carbon,intake</t>
+          <t>BMW F1X M6 Full Black Carbon intake</t>
         </is>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>BMW,F1X,M6,Full,Black,Carbon,intake</t>
+          <t>BMW F1X M6 Full Black Carbon intake</t>
         </is>
       </c>
       <c r="R60" t="inlineStr">
@@ -6548,12 +6548,12 @@
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>BMW,F40,M135i,,F44,M235i</t>
+          <t>BMW F40 M135i, F44 M235i</t>
         </is>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>BMW,F40,M135i,,F44,M235i</t>
+          <t>BMW F40 M135i, F44 M235i</t>
         </is>
       </c>
       <c r="R61" t="inlineStr">
@@ -6623,12 +6623,12 @@
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>BMW,F87,M2,Competition,Black,Carbon,intake</t>
+          <t>BMW F87 M2 Competition Black Carbon intake</t>
         </is>
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>BMW,F87,M2,Competition,Black,Carbon,intake</t>
+          <t>BMW F87 M2 Competition Black Carbon intake</t>
         </is>
       </c>
       <c r="R62" t="inlineStr">
@@ -6700,12 +6700,12 @@
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>V2,BMW,F87,M2,,F2X,M135i,,M235i,,F3X,335i,,435i,Carbon,intake</t>
+          <t>V2 BMW F87 M2, F2X M135i, M235i, F3X 335i, 435i Carbon intake</t>
         </is>
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>V2,BMW,F87,M2,,F2X,M135i,,M235i,,F3X,335i,,435i,Carbon,intake</t>
+          <t>V2 BMW F87 M2, F2X M135i, M235i, F3X 335i, 435i Carbon intake</t>
         </is>
       </c>
       <c r="R63" t="inlineStr">
@@ -6775,12 +6775,12 @@
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>BMW,N55,Black,Carbon,Engine,Cover</t>
+          <t>BMW N55 Black Carbon Engine Cover</t>
         </is>
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>BMW,N55,Black,Carbon,Engine,Cover</t>
+          <t>BMW N55 Black Carbon Engine Cover</t>
         </is>
       </c>
       <c r="R64" t="inlineStr">
@@ -6850,12 +6850,12 @@
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>BMW,F87,M2,Black,Carbon,Engine,Cover</t>
+          <t>BMW F87 M2 Black Carbon Engine Cover</t>
         </is>
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>BMW,F87,M2,Black,Carbon,Engine,Cover</t>
+          <t>BMW F87 M2 Black Carbon Engine Cover</t>
         </is>
       </c>
       <c r="R65" t="inlineStr">
@@ -6925,12 +6925,12 @@
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>BMW,F9X,X3M/X4M,Carbon,Intake,System</t>
+          <t>BMW F9X X3M/X4M Carbon Intake System</t>
         </is>
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>BMW,F9X,X3M/X4M,Carbon,Intake,System</t>
+          <t>BMW F9X X3M/X4M Carbon Intake System</t>
         </is>
       </c>
       <c r="R66" t="inlineStr">
@@ -7000,12 +7000,12 @@
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>BMW,F9X,X3M/X4M,Carbon,Intake,System,-,LCI,Version</t>
+          <t>BMW F9X X3M/X4M Carbon Intake System - LCI Version</t>
         </is>
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>BMW,F9X,X3M/X4M,Carbon,Intake,System,-,LCI,Version</t>
+          <t>BMW F9X X3M/X4M Carbon Intake System - LCI Version</t>
         </is>
       </c>
       <c r="R67" t="inlineStr">
@@ -7075,12 +7075,12 @@
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>BMW,Z4M,Black,Carbon,intake</t>
+          <t>BMW Z4M Black Carbon intake</t>
         </is>
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>BMW,Z4M,Black,Carbon,intake</t>
+          <t>BMW Z4M Black Carbon intake</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
@@ -7150,12 +7150,12 @@
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>BMW,G20,B48/B46,Intake,System,-,Pre,2018,November</t>
+          <t>BMW G20 B48/B46 Intake System - Pre 2018 November</t>
         </is>
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>BMW,G20,B48/B46,Intake,System,-,Pre,2018,November</t>
+          <t>BMW G20 B48/B46 Intake System - Pre 2018 November</t>
         </is>
       </c>
       <c r="R69" t="inlineStr">
@@ -7225,12 +7225,12 @@
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>BMW,G20/G42,B48/B46,Intake,System,-,Post,2018,November</t>
+          <t>BMW G20/G42 B48/B46 Intake System - Post 2018 November</t>
         </is>
       </c>
       <c r="Q70" t="inlineStr">
         <is>
-          <t>BMW,G20/G42,B48/B46,Intake,System,-,Post,2018,November</t>
+          <t>BMW G20/G42 B48/B46 Intake System - Post 2018 November</t>
         </is>
       </c>
       <c r="R70" t="inlineStr">
@@ -7300,12 +7300,12 @@
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>BMW,G20,B58,Intake,System,-,Pre,2018,November</t>
+          <t>BMW G20 B58 Intake System - Pre 2018 November</t>
         </is>
       </c>
       <c r="Q71" t="inlineStr">
         <is>
-          <t>BMW,G20,B58,Intake,System,-,Pre,2018,November</t>
+          <t>BMW G20 B58 Intake System - Pre 2018 November</t>
         </is>
       </c>
       <c r="R71" t="inlineStr">
@@ -7375,12 +7375,12 @@
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>BMW,G20/G42,B58,Intake,System,-,Post,2018,November</t>
+          <t>BMW G20/G42 B58 Intake System - Post 2018 November</t>
         </is>
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>BMW,G20/G42,B58,Intake,System,-,Post,2018,November</t>
+          <t>BMW G20/G42 B58 Intake System - Post 2018 November</t>
         </is>
       </c>
       <c r="R72" t="inlineStr">
@@ -7452,12 +7452,12 @@
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>BMW,G20,,G29,Z4,,B48,Engine,Cover</t>
+          <t>BMW G20, G29 Z4, B48 Engine Cover</t>
         </is>
       </c>
       <c r="Q73" t="inlineStr">
         <is>
-          <t>BMW,G20,,G29,Z4,,B48,Engine,Cover</t>
+          <t>BMW G20, G29 Z4, B48 Engine Cover</t>
         </is>
       </c>
       <c r="R73" t="inlineStr">
@@ -7527,12 +7527,12 @@
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>BMW,G29,Z4,M40i,B58,Carbon,Intake</t>
+          <t>BMW G29 Z4 M40i B58 Carbon Intake</t>
         </is>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>BMW,G29,Z4,M40i,B58,Carbon,Intake</t>
+          <t>BMW G29 Z4 M40i B58 Carbon Intake</t>
         </is>
       </c>
       <c r="R74" t="inlineStr">
@@ -7602,12 +7602,12 @@
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>BMW,G29,Z4,2.0,B48,Carbon,Intake</t>
+          <t>BMW G29 Z4 2.0 B48 Carbon Intake</t>
         </is>
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>BMW,G29,Z4,2.0,B48,Carbon,Intake</t>
+          <t>BMW G29 Z4 2.0 B48 Carbon Intake</t>
         </is>
       </c>
       <c r="R75" t="inlineStr">
@@ -7677,12 +7677,12 @@
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>BMW,G8X,M3/M4/CSL,Carbon,Engine,Cover,-,Gloss,Finish</t>
+          <t>BMW G8X M3/M4/CSL Carbon Engine Cover - Gloss Finish</t>
         </is>
       </c>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>BMW,G8X,M3/M4/CSL,Carbon,Engine,Cover,-,Gloss,Finish</t>
+          <t>BMW G8X M3/M4/CSL Carbon Engine Cover - Gloss Finish</t>
         </is>
       </c>
       <c r="R76" t="inlineStr">
@@ -7752,12 +7752,12 @@
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>BMW,G8X,M3/M4/CSL,Carbon,Engine,Cover,-,Matte,Finish</t>
+          <t>BMW G8X M3/M4/CSL Carbon Engine Cover - Matte Finish</t>
         </is>
       </c>
       <c r="Q77" t="inlineStr">
         <is>
-          <t>BMW,G8X,M3/M4/CSL,Carbon,Engine,Cover,-,Matte,Finish</t>
+          <t>BMW G8X M3/M4/CSL Carbon Engine Cover - Matte Finish</t>
         </is>
       </c>
       <c r="R77" t="inlineStr">
@@ -7827,12 +7827,12 @@
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>BMW,G8X,M3/M4,Carbon,Intake,for,all,strut,braces,-,Gloss,Finish</t>
+          <t>BMW G8X M3/M4 Carbon Intake for all strut braces - Gloss Finish</t>
         </is>
       </c>
       <c r="Q78" t="inlineStr">
         <is>
-          <t>BMW,G8X,M3/M4,Carbon,Intake,for,all,strut,braces,-,Gloss,Finish</t>
+          <t>BMW G8X M3/M4 Carbon Intake for all strut braces - Gloss Finish</t>
         </is>
       </c>
       <c r="R78" t="inlineStr">
@@ -7902,12 +7902,12 @@
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>BMW,G8X,M3/M4,Carbon,Intake,for,all,strut,braces,-,Matte,Finish</t>
+          <t>BMW G8X M3/M4 Carbon Intake for all strut braces - Matte Finish</t>
         </is>
       </c>
       <c r="Q79" t="inlineStr">
         <is>
-          <t>BMW,G8X,M3/M4,Carbon,Intake,for,all,strut,braces,-,Matte,Finish</t>
+          <t>BMW G8X M3/M4 Carbon Intake for all strut braces - Matte Finish</t>
         </is>
       </c>
       <c r="R79" t="inlineStr">
@@ -7977,12 +7977,12 @@
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Conversion,kit,for,G8X,M3/M4,intake,for,CSL,Strut,Brace,-,Gloss</t>
+          <t>Conversion kit for G8X M3/M4 intake for CSL Strut Brace - Gloss</t>
         </is>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>Conversion,kit,for,G8X,M3/M4,intake,for,CSL,Strut,Brace,-,Gloss</t>
+          <t>Conversion kit for G8X M3/M4 intake for CSL Strut Brace - Gloss</t>
         </is>
       </c>
       <c r="R80" t="inlineStr">
@@ -8052,12 +8052,12 @@
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Conversion,kit,for,G8X,M3/M4,intake,for,CSL,Strut,Brace,-,Matte</t>
+          <t>Conversion kit for G8X M3/M4 intake for CSL Strut Brace - Matte</t>
         </is>
       </c>
       <c r="Q81" t="inlineStr">
         <is>
-          <t>Conversion,kit,for,G8X,M3/M4,intake,for,CSL,Strut,Brace,-,Matte</t>
+          <t>Conversion kit for G8X M3/M4 intake for CSL Strut Brace - Matte</t>
         </is>
       </c>
       <c r="R81" t="inlineStr">
@@ -8127,12 +8127,12 @@
       </c>
       <c r="P82" t="inlineStr">
         <is>
-          <t>C8,Corvette,Stingray,Coupe,Carbon,Intake,</t>
+          <t xml:space="preserve">C8 Corvette Stingray Coupe Carbon Intake </t>
         </is>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>C8,Corvette,Stingray,Coupe,Carbon,Intake,</t>
+          <t xml:space="preserve">C8 Corvette Stingray Coupe Carbon Intake </t>
         </is>
       </c>
       <c r="R82" t="inlineStr">
@@ -8202,12 +8202,12 @@
       </c>
       <c r="P83" t="inlineStr">
         <is>
-          <t>C8,Corvette,Stingray,Hard,Top,Convertible,Carbon,Intake,</t>
+          <t xml:space="preserve">C8 Corvette Stingray Hard Top Convertible Carbon Intake </t>
         </is>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>C8,Corvette,Stingray,Hard,Top,Convertible,Carbon,Intake,</t>
+          <t xml:space="preserve">C8 Corvette Stingray Hard Top Convertible Carbon Intake </t>
         </is>
       </c>
       <c r="R83" t="inlineStr">
@@ -8277,12 +8277,12 @@
       </c>
       <c r="P84" t="inlineStr">
         <is>
-          <t>C8,Corvette,Stingray,Carbon,Engine,Cover,</t>
+          <t xml:space="preserve">C8 Corvette Stingray Carbon Engine Cover </t>
         </is>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>C8,Corvette,Stingray,Carbon,Engine,Cover,</t>
+          <t xml:space="preserve">C8 Corvette Stingray Carbon Engine Cover </t>
         </is>
       </c>
       <c r="R84" t="inlineStr">
@@ -8352,12 +8352,12 @@
       </c>
       <c r="P85" t="inlineStr">
         <is>
-          <t>Honda,FK2,Black,Carbon,MAF-TUBE,and,silicone,hose</t>
+          <t>Honda FK2 Black Carbon MAF-TUBE and silicone hose</t>
         </is>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>Honda,FK2,Black,Carbon,MAF-TUBE,and,silicone,hose</t>
+          <t>Honda FK2 Black Carbon MAF-TUBE and silicone hose</t>
         </is>
       </c>
       <c r="R85" t="inlineStr">
@@ -8427,12 +8427,12 @@
       </c>
       <c r="P86" t="inlineStr">
         <is>
-          <t>V2,FK2,Civic,Type,R,LHD,Carbon,intake,with,upgraded,Carbon,Tube</t>
+          <t>V2 FK2 Civic Type R LHD Carbon intake with upgraded Carbon Tube</t>
         </is>
       </c>
       <c r="Q86" t="inlineStr">
         <is>
-          <t>V2,FK2,Civic,Type,R,LHD,Carbon,intake,with,upgraded,Carbon,Tube</t>
+          <t>V2 FK2 Civic Type R LHD Carbon intake with upgraded Carbon Tube</t>
         </is>
       </c>
       <c r="R86" t="inlineStr">
@@ -8503,12 +8503,12 @@
       </c>
       <c r="P87" t="inlineStr">
         <is>
-          <t>V2,FK2,Civic,Type,R,RHD,Carbon,intake,with,upgraded,Carbon,Tube</t>
+          <t>V2 FK2 Civic Type R RHD Carbon intake with upgraded Carbon Tube</t>
         </is>
       </c>
       <c r="Q87" t="inlineStr">
         <is>
-          <t>V2,FK2,Civic,Type,R,RHD,Carbon,intake,with,upgraded,Carbon,Tube</t>
+          <t>V2 FK2 Civic Type R RHD Carbon intake with upgraded Carbon Tube</t>
         </is>
       </c>
       <c r="R87" t="inlineStr">
@@ -8578,12 +8578,12 @@
       </c>
       <c r="P88" t="inlineStr">
         <is>
-          <t>FK8,and,FK2,Engine,Cover,Red,and,Black</t>
+          <t>FK8 and FK2 Engine Cover Red and Black</t>
         </is>
       </c>
       <c r="Q88" t="inlineStr">
         <is>
-          <t>FK8,and,FK2,Engine,Cover,Red,and,Black</t>
+          <t>FK8 and FK2 Engine Cover Red and Black</t>
         </is>
       </c>
       <c r="R88" t="inlineStr">
@@ -8653,12 +8653,12 @@
       </c>
       <c r="P89" t="inlineStr">
         <is>
-          <t>FK2,Carbon,Turbo,Tube,for,Customers,with,FK2,V2,Intake</t>
+          <t>FK2 Carbon Turbo Tube for Customers with FK2 V2 Intake</t>
         </is>
       </c>
       <c r="Q89" t="inlineStr">
         <is>
-          <t>FK2,Carbon,Turbo,Tube,for,Customers,with,FK2,V2,Intake</t>
+          <t>FK2 Carbon Turbo Tube for Customers with FK2 V2 Intake</t>
         </is>
       </c>
       <c r="R89" t="inlineStr">
@@ -8728,12 +8728,12 @@
       </c>
       <c r="P90" t="inlineStr">
         <is>
-          <t>FK2,Carbon,Turbo,Tube,Package,with,V2,MAF,Tube</t>
+          <t>FK2 Carbon Turbo Tube Package with V2 MAF Tube</t>
         </is>
       </c>
       <c r="Q90" t="inlineStr">
         <is>
-          <t>FK2,Carbon,Turbo,Tube,Package,with,V2,MAF,Tube</t>
+          <t>FK2 Carbon Turbo Tube Package with V2 MAF Tube</t>
         </is>
       </c>
       <c r="R90" t="inlineStr">
@@ -8803,12 +8803,12 @@
       </c>
       <c r="P91" t="inlineStr">
         <is>
-          <t>FK8,Civic,Type,R,Black,Carbon,intake</t>
+          <t>FK8 Civic Type R Black Carbon intake</t>
         </is>
       </c>
       <c r="Q91" t="inlineStr">
         <is>
-          <t>FK8,Civic,Type,R,Black,Carbon,intake</t>
+          <t>FK8 Civic Type R Black Carbon intake</t>
         </is>
       </c>
       <c r="R91" t="inlineStr">
@@ -8878,12 +8878,12 @@
       </c>
       <c r="P92" t="inlineStr">
         <is>
-          <t>FK8,Carbon,V2,MAF,Tube,and,Silicon,Set</t>
+          <t>FK8 Carbon V2 MAF Tube and Silicon Set</t>
         </is>
       </c>
       <c r="Q92" t="inlineStr">
         <is>
-          <t>FK8,Carbon,V2,MAF,Tube,and,Silicon,Set</t>
+          <t>FK8 Carbon V2 MAF Tube and Silicon Set</t>
         </is>
       </c>
       <c r="R92" t="inlineStr">
@@ -8953,12 +8953,12 @@
       </c>
       <c r="P93" t="inlineStr">
         <is>
-          <t>FK8,and,FK2,Engine,Cover,Red,and,Black</t>
+          <t>FK8 and FK2 Engine Cover Red and Black</t>
         </is>
       </c>
       <c r="Q93" t="inlineStr">
         <is>
-          <t>FK8,and,FK2,Engine,Cover,Red,and,Black</t>
+          <t>FK8 and FK2 Engine Cover Red and Black</t>
         </is>
       </c>
       <c r="R93" t="inlineStr">
@@ -9028,12 +9028,12 @@
       </c>
       <c r="P94" t="inlineStr">
         <is>
-          <t>FK8,Carbon,Turbo,Tube,for,customers,with,V2,MAF,tube</t>
+          <t>FK8 Carbon Turbo Tube for customers with V2 MAF tube</t>
         </is>
       </c>
       <c r="Q94" t="inlineStr">
         <is>
-          <t>FK8,Carbon,Turbo,Tube,for,customers,with,V2,MAF,tube</t>
+          <t>FK8 Carbon Turbo Tube for customers with V2 MAF tube</t>
         </is>
       </c>
       <c r="R94" t="inlineStr">
@@ -9103,12 +9103,12 @@
       </c>
       <c r="P95" t="inlineStr">
         <is>
-          <t>FK8,Carbon,Turbo,Tube,Package,with,V2,MAF,Tube</t>
+          <t>FK8 Carbon Turbo Tube Package with V2 MAF Tube</t>
         </is>
       </c>
       <c r="Q95" t="inlineStr">
         <is>
-          <t>FK8,Carbon,Turbo,Tube,Package,with,V2,MAF,Tube</t>
+          <t>FK8 Carbon Turbo Tube Package with V2 MAF Tube</t>
         </is>
       </c>
       <c r="R95" t="inlineStr">
@@ -9178,12 +9178,12 @@
       </c>
       <c r="P96" t="inlineStr">
         <is>
-          <t>Lamborghini,Huracan,Carbon,Intake</t>
+          <t>Lamborghini Huracan Carbon Intake</t>
         </is>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
-          <t>Lamborghini,Huracan,Carbon,Intake</t>
+          <t>Lamborghini Huracan Carbon Intake</t>
         </is>
       </c>
       <c r="R96" t="inlineStr">
@@ -9255,12 +9255,12 @@
       </c>
       <c r="P97" t="inlineStr">
         <is>
-          <t>Lamborghini,Huracan,Carbon,Engine,Cover,Set,Matte,Finish</t>
+          <t>Lamborghini Huracan Carbon Engine Cover Set Matte Finish</t>
         </is>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
-          <t>Lamborghini,Huracan,Carbon,Engine,Cover,Set,Matte,Finish</t>
+          <t>Lamborghini Huracan Carbon Engine Cover Set Matte Finish</t>
         </is>
       </c>
       <c r="R97" t="inlineStr">
@@ -9330,12 +9330,12 @@
       </c>
       <c r="P98" t="inlineStr">
         <is>
-          <t>Lamborghini,Urus,Intake,System</t>
+          <t>Lamborghini Urus Intake System</t>
         </is>
       </c>
       <c r="Q98" t="inlineStr">
         <is>
-          <t>Lamborghini,Urus,Intake,System</t>
+          <t>Lamborghini Urus Intake System</t>
         </is>
       </c>
       <c r="R98" t="inlineStr">
@@ -9405,12 +9405,12 @@
       </c>
       <c r="P99" t="inlineStr">
         <is>
-          <t>Mercedes,A35,AMG,,GLA35,,GLB35,,A250,Carbon,Intake</t>
+          <t>Mercedes A35 AMG, GLA35, GLB35, A250 Carbon Intake</t>
         </is>
       </c>
       <c r="Q99" t="inlineStr">
         <is>
-          <t>Mercedes,A35,AMG,,GLA35,,GLB35,,A250,Carbon,Intake</t>
+          <t>Mercedes A35 AMG, GLA35, GLB35, A250 Carbon Intake</t>
         </is>
       </c>
       <c r="R99" t="inlineStr">
@@ -9482,12 +9482,12 @@
       </c>
       <c r="P100" t="inlineStr">
         <is>
-          <t>Mercedes,A35,AMG,,GLA35,,GLB35,,Turbo,Tube</t>
+          <t>Mercedes A35 AMG, GLA35, GLB35, Turbo Tube</t>
         </is>
       </c>
       <c r="Q100" t="inlineStr">
         <is>
-          <t>Mercedes,A35,AMG,,GLA35,,GLB35,,Turbo,Tube</t>
+          <t>Mercedes A35 AMG, GLA35, GLB35, Turbo Tube</t>
         </is>
       </c>
       <c r="R100" t="inlineStr">
@@ -9557,12 +9557,12 @@
       </c>
       <c r="P101" t="inlineStr">
         <is>
-          <t>Mercedes,A45S,CLA45S,GLA45,GLB45,AMG,Carbon,Intake,</t>
+          <t xml:space="preserve">Mercedes A45S CLA45S GLA45 GLB45 AMG Carbon Intake </t>
         </is>
       </c>
       <c r="Q101" t="inlineStr">
         <is>
-          <t>Mercedes,A45S,CLA45S,GLA45,GLB45,AMG,Carbon,Intake,</t>
+          <t xml:space="preserve">Mercedes A45S CLA45S GLA45 GLB45 AMG Carbon Intake </t>
         </is>
       </c>
       <c r="R101" t="inlineStr">
@@ -9632,12 +9632,12 @@
       </c>
       <c r="P102" t="inlineStr">
         <is>
-          <t>Mercedes,C190/R190,AMG,GTR,,GTS,,GT,GLOSS,Finish</t>
+          <t>Mercedes C190/R190 AMG GTR, GTS, GT GLOSS Finish</t>
         </is>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>Mercedes,C190/R190,AMG,GTR,,GTS,,GT,GLOSS,Finish</t>
+          <t>Mercedes C190/R190 AMG GTR, GTS, GT GLOSS Finish</t>
         </is>
       </c>
       <c r="R102" t="inlineStr">
@@ -9707,12 +9707,12 @@
       </c>
       <c r="P103" t="inlineStr">
         <is>
-          <t>Mercedes,C190/R190,AMG,GTR,,GTS,,GT,MATTE,Finish</t>
+          <t>Mercedes C190/R190 AMG GTR, GTS, GT MATTE Finish</t>
         </is>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>Mercedes,C190/R190,AMG,GTR,,GTS,,GT,MATTE,Finish</t>
+          <t>Mercedes C190/R190 AMG GTR, GTS, GT MATTE Finish</t>
         </is>
       </c>
       <c r="R103" t="inlineStr">
@@ -9784,12 +9784,12 @@
       </c>
       <c r="P104" t="inlineStr">
         <is>
-          <t>Mercedes,all,X205,C63/C63S,variants,,AMG,Carbon,intake</t>
+          <t>Mercedes all X205 C63/C63S variants, AMG Carbon intake</t>
         </is>
       </c>
       <c r="Q104" t="inlineStr">
         <is>
-          <t>Mercedes,all,X205,C63/C63S,variants,,AMG,Carbon,intake</t>
+          <t>Mercedes all X205 C63/C63S variants, AMG Carbon intake</t>
         </is>
       </c>
       <c r="R104" t="inlineStr">
@@ -9859,12 +9859,12 @@
       </c>
       <c r="P105" t="inlineStr">
         <is>
-          <t>C63S,Carbon,Duct,upgrade,package</t>
+          <t>C63S Carbon Duct upgrade package</t>
         </is>
       </c>
       <c r="Q105" t="inlineStr">
         <is>
-          <t>C63S,Carbon,Duct,upgrade,package</t>
+          <t>C63S Carbon Duct upgrade package</t>
         </is>
       </c>
       <c r="R105" t="inlineStr">
@@ -9936,12 +9936,12 @@
       </c>
       <c r="P106" t="inlineStr">
         <is>
-          <t>Mercedes,GLC63S,carbon,intake,</t>
+          <t xml:space="preserve">Mercedes GLC63S carbon intake </t>
         </is>
       </c>
       <c r="Q106" t="inlineStr">
         <is>
-          <t>Mercedes,GLC63S,carbon,intake,</t>
+          <t xml:space="preserve">Mercedes GLC63S carbon intake </t>
         </is>
       </c>
       <c r="R106" t="inlineStr">
@@ -10013,12 +10013,12 @@
       </c>
       <c r="P107" t="inlineStr">
         <is>
-          <t>Mini,JCW,GP3,/,Clubman,/,JCW,306HP,Carbon,Intake</t>
+          <t>Mini JCW GP3 / Clubman / JCW 306HP Carbon Intake</t>
         </is>
       </c>
       <c r="Q107" t="inlineStr">
         <is>
-          <t>Mini,JCW,GP3,/,Clubman,/,JCW,306HP,Carbon,Intake</t>
+          <t>Mini JCW GP3 / Clubman / JCW 306HP Carbon Intake</t>
         </is>
       </c>
       <c r="R107" t="inlineStr">
@@ -10088,12 +10088,12 @@
       </c>
       <c r="P108" t="inlineStr">
         <is>
-          <t>Mini,JCW,Countryman,306HP,Carbon,Intake,with,no,scoop</t>
+          <t>Mini JCW Countryman 306HP Carbon Intake with no scoop</t>
         </is>
       </c>
       <c r="Q108" t="inlineStr">
         <is>
-          <t>Mini,JCW,Countryman,306HP,Carbon,Intake,with,no,scoop</t>
+          <t>Mini JCW Countryman 306HP Carbon Intake with no scoop</t>
         </is>
       </c>
       <c r="R108" t="inlineStr">
@@ -10165,12 +10165,12 @@
       </c>
       <c r="P109" t="inlineStr">
         <is>
-          <t>Mini,Cooper,S,/,JCW,Black,Carbon,intake</t>
+          <t>Mini Cooper S / JCW Black Carbon intake</t>
         </is>
       </c>
       <c r="Q109" t="inlineStr">
         <is>
-          <t>Mini,Cooper,S,/,JCW,Black,Carbon,intake</t>
+          <t>Mini Cooper S / JCW Black Carbon intake</t>
         </is>
       </c>
       <c r="R109" t="inlineStr">
@@ -10242,12 +10242,12 @@
       </c>
       <c r="P110" t="inlineStr">
         <is>
-          <t>Mini,Cooper,S,/,JCW,Facelift,Black,Carbon,intake</t>
+          <t>Mini Cooper S / JCW Facelift Black Carbon intake</t>
         </is>
       </c>
       <c r="Q110" t="inlineStr">
         <is>
-          <t>Mini,Cooper,S,/,JCW,Facelift,Black,Carbon,intake</t>
+          <t>Mini Cooper S / JCW Facelift Black Carbon intake</t>
         </is>
       </c>
       <c r="R110" t="inlineStr">
@@ -10317,12 +10317,12 @@
       </c>
       <c r="P111" t="inlineStr">
         <is>
-          <t>Mini,Cooper,S,/,JCW,Plastic,intake,with,Carbon,Scoop</t>
+          <t>Mini Cooper S / JCW Plastic intake with Carbon Scoop</t>
         </is>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>Mini,Cooper,S,/,JCW,Plastic,intake,with,Carbon,Scoop</t>
+          <t>Mini Cooper S / JCW Plastic intake with Carbon Scoop</t>
         </is>
       </c>
       <c r="R111" t="inlineStr">
@@ -10392,12 +10392,12 @@
       </c>
       <c r="P112" t="inlineStr">
         <is>
-          <t>Mini,Cooper,S,/,JCW,Facelift,Plastic,intake,with,Carbon,Scoop</t>
+          <t>Mini Cooper S / JCW Facelift Plastic intake with Carbon Scoop</t>
         </is>
       </c>
       <c r="Q112" t="inlineStr">
         <is>
-          <t>Mini,Cooper,S,/,JCW,Facelift,Plastic,intake,with,Carbon,Scoop</t>
+          <t>Mini Cooper S / JCW Facelift Plastic intake with Carbon Scoop</t>
         </is>
       </c>
       <c r="R112" t="inlineStr">
@@ -10467,12 +10467,12 @@
       </c>
       <c r="P113" t="inlineStr">
         <is>
-          <t>MINI,Countryman,S,Black,Carbon,intake,with,no,scoop</t>
+          <t>MINI Countryman S Black Carbon intake with no scoop</t>
         </is>
       </c>
       <c r="Q113" t="inlineStr">
         <is>
-          <t>MINI,Countryman,S,Black,Carbon,intake,with,no,scoop</t>
+          <t>MINI Countryman S Black Carbon intake with no scoop</t>
         </is>
       </c>
       <c r="R113" t="inlineStr">
@@ -10542,12 +10542,12 @@
       </c>
       <c r="P114" t="inlineStr">
         <is>
-          <t>MINI,Countryman,S,Facelift,Black,Carbon,intake,with,no,scoop</t>
+          <t>MINI Countryman S Facelift Black Carbon intake with no scoop</t>
         </is>
       </c>
       <c r="Q114" t="inlineStr">
         <is>
-          <t>MINI,Countryman,S,Facelift,Black,Carbon,intake,with,no,scoop</t>
+          <t>MINI Countryman S Facelift Black Carbon intake with no scoop</t>
         </is>
       </c>
       <c r="R114" t="inlineStr">
@@ -10617,12 +10617,12 @@
       </c>
       <c r="P115" t="inlineStr">
         <is>
-          <t>MINI,Countryman,S,Plastic,intake,with,no,scoop</t>
+          <t>MINI Countryman S Plastic intake with no scoop</t>
         </is>
       </c>
       <c r="Q115" t="inlineStr">
         <is>
-          <t>MINI,Countryman,S,Plastic,intake,with,no,scoop</t>
+          <t>MINI Countryman S Plastic intake with no scoop</t>
         </is>
       </c>
       <c r="R115" t="inlineStr">
@@ -10692,12 +10692,12 @@
       </c>
       <c r="P116" t="inlineStr">
         <is>
-          <t>MINI,Countryman,S,Facelift,Plastic,intake,with,no,scoop</t>
+          <t>MINI Countryman S Facelift Plastic intake with no scoop</t>
         </is>
       </c>
       <c r="Q116" t="inlineStr">
         <is>
-          <t>MINI,Countryman,S,Facelift,Plastic,intake,with,no,scoop</t>
+          <t>MINI Countryman S Facelift Plastic intake with no scoop</t>
         </is>
       </c>
       <c r="R116" t="inlineStr">
@@ -10767,12 +10767,12 @@
       </c>
       <c r="P117" t="inlineStr">
         <is>
-          <t>Porsche,991,Turbo,Black,Carbon,intake</t>
+          <t>Porsche 991 Turbo Black Carbon intake</t>
         </is>
       </c>
       <c r="Q117" t="inlineStr">
         <is>
-          <t>Porsche,991,Turbo,Black,Carbon,intake</t>
+          <t>Porsche 991 Turbo Black Carbon intake</t>
         </is>
       </c>
       <c r="R117" t="inlineStr">
@@ -10842,12 +10842,12 @@
       </c>
       <c r="P118" t="inlineStr">
         <is>
-          <t>Porsche,991.1,991.2,GT3RS,Carbon,Intake</t>
+          <t>Porsche 991.1 991.2 GT3RS Carbon Intake</t>
         </is>
       </c>
       <c r="Q118" t="inlineStr">
         <is>
-          <t>Porsche,991.1,991.2,GT3RS,Carbon,Intake</t>
+          <t>Porsche 991.1 991.2 GT3RS Carbon Intake</t>
         </is>
       </c>
       <c r="R118" t="inlineStr">
@@ -10917,12 +10917,12 @@
       </c>
       <c r="P119" t="inlineStr">
         <is>
-          <t>Porsche,Cayenne,2020+,GTS,,2019+,Turbo,S,4.0,TFSI,Intake</t>
+          <t>Porsche Cayenne 2020+ GTS, 2019+ Turbo S 4.0 TFSI Intake</t>
         </is>
       </c>
       <c r="Q119" t="inlineStr">
         <is>
-          <t>Porsche,Cayenne,2020+,GTS,,2019+,Turbo,S,4.0,TFSI,Intake</t>
+          <t>Porsche Cayenne 2020+ GTS, 2019+ Turbo S 4.0 TFSI Intake</t>
         </is>
       </c>
       <c r="R119" t="inlineStr">
@@ -10994,12 +10994,12 @@
       </c>
       <c r="P120" t="inlineStr">
         <is>
-          <t>Leon,Cupra,2.0,TFSI-,Full,Black,Carbon,intake</t>
+          <t>Leon Cupra 2.0 TFSI- Full Black Carbon intake</t>
         </is>
       </c>
       <c r="Q120" t="inlineStr">
         <is>
-          <t>Leon,Cupra,2.0,TFSI-,Full,Black,Carbon,intake</t>
+          <t>Leon Cupra 2.0 TFSI- Full Black Carbon intake</t>
         </is>
       </c>
       <c r="R120" t="inlineStr">
@@ -11069,12 +11069,12 @@
       </c>
       <c r="P121" t="inlineStr">
         <is>
-          <t>MK4,Leon,Cupra,Formentor,2.0,VZ1,245hp,2020+,Carbon,intake</t>
+          <t>MK4 Leon Cupra Formentor 2.0 VZ1 245hp 2020+ Carbon intake</t>
         </is>
       </c>
       <c r="Q121" t="inlineStr">
         <is>
-          <t>MK4,Leon,Cupra,Formentor,2.0,VZ1,245hp,2020+,Carbon,intake</t>
+          <t>MK4 Leon Cupra Formentor 2.0 VZ1 245hp 2020+ Carbon intake</t>
         </is>
       </c>
       <c r="R121" t="inlineStr">
@@ -11144,12 +11144,12 @@
       </c>
       <c r="P122" t="inlineStr">
         <is>
-          <t>MK4,Leon,Cupra,Formentor,2.0,VZ2,300hp,2020+,Carbon,intake</t>
+          <t>MK4 Leon Cupra Formentor 2.0 VZ2 300hp 2020+ Carbon intake</t>
         </is>
       </c>
       <c r="Q122" t="inlineStr">
         <is>
-          <t>MK4,Leon,Cupra,Formentor,2.0,VZ2,300hp,2020+,Carbon,intake</t>
+          <t>MK4 Leon Cupra Formentor 2.0 VZ2 300hp 2020+ Carbon intake</t>
         </is>
       </c>
       <c r="R122" t="inlineStr">
@@ -11221,12 +11221,12 @@
       </c>
       <c r="P123" t="inlineStr">
         <is>
-          <t>MK4,Leon,Cupra,Formentor,2.5,VZ5,390hp,2020+,Carbon,intake</t>
+          <t>MK4 Leon Cupra Formentor 2.5 VZ5 390hp 2020+ Carbon intake</t>
         </is>
       </c>
       <c r="Q123" t="inlineStr">
         <is>
-          <t>MK4,Leon,Cupra,Formentor,2.5,VZ5,390hp,2020+,Carbon,intake</t>
+          <t>MK4 Leon Cupra Formentor 2.5 VZ5 390hp 2020+ Carbon intake</t>
         </is>
       </c>
       <c r="R123" t="inlineStr">
@@ -11296,12 +11296,12 @@
       </c>
       <c r="P124" t="inlineStr">
         <is>
-          <t>Toyota,MK5,3.0,B58,Supra,Carbon,Intake</t>
+          <t>Toyota MK5 3.0 B58 Supra Carbon Intake</t>
         </is>
       </c>
       <c r="Q124" t="inlineStr">
         <is>
-          <t>Toyota,MK5,3.0,B58,Supra,Carbon,Intake</t>
+          <t>Toyota MK5 3.0 B58 Supra Carbon Intake</t>
         </is>
       </c>
       <c r="R124" t="inlineStr">
@@ -11371,12 +11371,12 @@
       </c>
       <c r="P125" t="inlineStr">
         <is>
-          <t>Toyota,MK5,2.0,B48,Supra,Carbon,Intake</t>
+          <t>Toyota MK5 2.0 B48 Supra Carbon Intake</t>
         </is>
       </c>
       <c r="Q125" t="inlineStr">
         <is>
-          <t>Toyota,MK5,2.0,B48,Supra,Carbon,Intake</t>
+          <t>Toyota MK5 2.0 B48 Supra Carbon Intake</t>
         </is>
       </c>
       <c r="R125" t="inlineStr">
@@ -11446,12 +11446,12 @@
       </c>
       <c r="P126" t="inlineStr">
         <is>
-          <t>Toyota,MK5,Supra,Carbon,Headlamp,Duct</t>
+          <t>Toyota MK5 Supra Carbon Headlamp Duct</t>
         </is>
       </c>
       <c r="Q126" t="inlineStr">
         <is>
-          <t>Toyota,MK5,Supra,Carbon,Headlamp,Duct</t>
+          <t>Toyota MK5 Supra Carbon Headlamp Duct</t>
         </is>
       </c>
       <c r="R126" t="inlineStr">
@@ -11523,12 +11523,12 @@
       </c>
       <c r="P127" t="inlineStr">
         <is>
-          <t>Toyota,MK5,Supra,Carbon,Engine,cover</t>
+          <t>Toyota MK5 Supra Carbon Engine cover</t>
         </is>
       </c>
       <c r="Q127" t="inlineStr">
         <is>
-          <t>Toyota,MK5,Supra,Carbon,Engine,cover</t>
+          <t>Toyota MK5 Supra Carbon Engine cover</t>
         </is>
       </c>
       <c r="R127" t="inlineStr">
@@ -11600,12 +11600,12 @@
       </c>
       <c r="P128" t="inlineStr">
         <is>
-          <t>Toyota,GR,Yaris/Corolla,Carbon,Engine,Cover,-,Gloss</t>
+          <t>Toyota GR Yaris/Corolla Carbon Engine Cover - Gloss</t>
         </is>
       </c>
       <c r="Q128" t="inlineStr">
         <is>
-          <t>Toyota,GR,Yaris/Corolla,Carbon,Engine,Cover,-,Gloss</t>
+          <t>Toyota GR Yaris/Corolla Carbon Engine Cover - Gloss</t>
         </is>
       </c>
       <c r="R128" t="inlineStr">
@@ -11677,12 +11677,12 @@
       </c>
       <c r="P129" t="inlineStr">
         <is>
-          <t>Toyota,GR,Yaris/Corolla,Carbon,Engine,Cover,-,Matte</t>
+          <t>Toyota GR Yaris/Corolla Carbon Engine Cover - Matte</t>
         </is>
       </c>
       <c r="Q129" t="inlineStr">
         <is>
-          <t>Toyota,GR,Yaris/Corolla,Carbon,Engine,Cover,-,Matte</t>
+          <t>Toyota GR Yaris/Corolla Carbon Engine Cover - Matte</t>
         </is>
       </c>
       <c r="R129" t="inlineStr">
@@ -11752,12 +11752,12 @@
       </c>
       <c r="P130" t="inlineStr">
         <is>
-          <t>Toyota,GR,Yaris,Carbon,Intake,-,Gloss</t>
+          <t>Toyota GR Yaris Carbon Intake - Gloss</t>
         </is>
       </c>
       <c r="Q130" t="inlineStr">
         <is>
-          <t>Toyota,GR,Yaris,Carbon,Intake,-,Gloss</t>
+          <t>Toyota GR Yaris Carbon Intake - Gloss</t>
         </is>
       </c>
       <c r="R130" t="inlineStr">
@@ -11827,12 +11827,12 @@
       </c>
       <c r="P131" t="inlineStr">
         <is>
-          <t>Toyota,GR,Yaris,Carbon,Intake,-,Matte</t>
+          <t>Toyota GR Yaris Carbon Intake - Matte</t>
         </is>
       </c>
       <c r="Q131" t="inlineStr">
         <is>
-          <t>Toyota,GR,Yaris,Carbon,Intake,-,Matte</t>
+          <t>Toyota GR Yaris Carbon Intake - Matte</t>
         </is>
       </c>
       <c r="R131" t="inlineStr">
@@ -11902,12 +11902,12 @@
       </c>
       <c r="P132" t="inlineStr">
         <is>
-          <t>Toyota,GR,Corolla,Carbon,Intake,-,Gloss</t>
+          <t>Toyota GR Corolla Carbon Intake - Gloss</t>
         </is>
       </c>
       <c r="Q132" t="inlineStr">
         <is>
-          <t>Toyota,GR,Corolla,Carbon,Intake,-,Gloss</t>
+          <t>Toyota GR Corolla Carbon Intake - Gloss</t>
         </is>
       </c>
       <c r="R132" t="inlineStr">
@@ -11977,12 +11977,12 @@
       </c>
       <c r="P133" t="inlineStr">
         <is>
-          <t>Toyota,GR,Corolla,Carbon,Intake,-,Matte</t>
+          <t>Toyota GR Corolla Carbon Intake - Matte</t>
         </is>
       </c>
       <c r="Q133" t="inlineStr">
         <is>
-          <t>Toyota,GR,Corolla,Carbon,Intake,-,Matte</t>
+          <t>Toyota GR Corolla Carbon Intake - Matte</t>
         </is>
       </c>
       <c r="R133" t="inlineStr">
@@ -12054,12 +12054,12 @@
       </c>
       <c r="P134" t="inlineStr">
         <is>
-          <t>Golf,MK7,GTi,,R,Carbon,intake</t>
+          <t>Golf MK7 GTi, R Carbon intake</t>
         </is>
       </c>
       <c r="Q134" t="inlineStr">
         <is>
-          <t>Golf,MK7,GTi,,R,Carbon,intake</t>
+          <t>Golf MK7 GTi, R Carbon intake</t>
         </is>
       </c>
       <c r="R134" t="inlineStr">
@@ -12129,12 +12129,12 @@
       </c>
       <c r="P135" t="inlineStr">
         <is>
-          <t>Golf,MK8,R,,Gti,Clubsport,Carbon,intake</t>
+          <t>Golf MK8 R, Gti Clubsport Carbon intake</t>
         </is>
       </c>
       <c r="Q135" t="inlineStr">
         <is>
-          <t>Golf,MK8,R,,Gti,Clubsport,Carbon,intake</t>
+          <t>Golf MK8 R, Gti Clubsport Carbon intake</t>
         </is>
       </c>
       <c r="R135" t="inlineStr">
@@ -12204,12 +12204,12 @@
       </c>
       <c r="P136" t="inlineStr">
         <is>
-          <t>Golf,MK8,Gti,Carbon,intake</t>
+          <t>Golf MK8 Gti Carbon intake</t>
         </is>
       </c>
       <c r="Q136" t="inlineStr">
         <is>
-          <t>Golf,MK8,Gti,Carbon,intake</t>
+          <t>Golf MK8 Gti Carbon intake</t>
         </is>
       </c>
       <c r="R136" t="inlineStr">
@@ -12279,12 +12279,12 @@
       </c>
       <c r="P137" t="inlineStr">
         <is>
-          <t>Golf,MK8,Engine,Cover</t>
+          <t>Golf MK8 Engine Cover</t>
         </is>
       </c>
       <c r="Q137" t="inlineStr">
         <is>
-          <t>Golf,MK8,Engine,Cover</t>
+          <t>Golf MK8 Engine Cover</t>
         </is>
       </c>
       <c r="R137" t="inlineStr">
@@ -12356,12 +12356,12 @@
       </c>
       <c r="P138" t="inlineStr">
         <is>
-          <t>Filter,Cleaning,Kit</t>
+          <t>Filter Cleaning Kit</t>
         </is>
       </c>
       <c r="Q138" t="inlineStr">
         <is>
-          <t>Filter,Cleaning,Kit</t>
+          <t>Filter Cleaning Kit</t>
         </is>
       </c>
       <c r="R138" t="inlineStr">
@@ -12433,12 +12433,12 @@
       </c>
       <c r="P139" t="inlineStr">
         <is>
-          <t>Replacement,Filter,TYPE,S</t>
+          <t>Replacement Filter TYPE S</t>
         </is>
       </c>
       <c r="Q139" t="inlineStr">
         <is>
-          <t>Replacement,Filter,TYPE,S</t>
+          <t>Replacement Filter TYPE S</t>
         </is>
       </c>
       <c r="R139" t="inlineStr">
@@ -12510,12 +12510,12 @@
       </c>
       <c r="P140" t="inlineStr">
         <is>
-          <t>Replacement,Filter,TYPE,B</t>
+          <t>Replacement Filter TYPE B</t>
         </is>
       </c>
       <c r="Q140" t="inlineStr">
         <is>
-          <t>Replacement,Filter,TYPE,B</t>
+          <t>Replacement Filter TYPE B</t>
         </is>
       </c>
       <c r="R140" t="inlineStr">
@@ -12587,12 +12587,12 @@
       </c>
       <c r="P141" t="inlineStr">
         <is>
-          <t>Replacement,Filter,TYPE,E</t>
+          <t>Replacement Filter TYPE E</t>
         </is>
       </c>
       <c r="Q141" t="inlineStr">
         <is>
-          <t>Replacement,Filter,TYPE,E</t>
+          <t>Replacement Filter TYPE E</t>
         </is>
       </c>
       <c r="R141" t="inlineStr">
@@ -12662,12 +12662,12 @@
       </c>
       <c r="P142" t="inlineStr">
         <is>
-          <t>Replacement,Filter,TYPE,D</t>
+          <t>Replacement Filter TYPE D</t>
         </is>
       </c>
       <c r="Q142" t="inlineStr">
         <is>
-          <t>Replacement,Filter,TYPE,D</t>
+          <t>Replacement Filter TYPE D</t>
         </is>
       </c>
       <c r="R142" t="inlineStr">
@@ -12739,12 +12739,12 @@
       </c>
       <c r="P143" t="inlineStr">
         <is>
-          <t>Replacement,Filter,TYPE,L</t>
+          <t>Replacement Filter TYPE L</t>
         </is>
       </c>
       <c r="Q143" t="inlineStr">
         <is>
-          <t>Replacement,Filter,TYPE,L</t>
+          <t>Replacement Filter TYPE L</t>
         </is>
       </c>
       <c r="R143" t="inlineStr">
@@ -12814,12 +12814,12 @@
       </c>
       <c r="P144" t="inlineStr">
         <is>
-          <t>Replacement,Filter,TYPE,D2</t>
+          <t>Replacement Filter TYPE D2</t>
         </is>
       </c>
       <c r="Q144" t="inlineStr">
         <is>
-          <t>Replacement,Filter,TYPE,D2</t>
+          <t>Replacement Filter TYPE D2</t>
         </is>
       </c>
       <c r="R144" t="inlineStr">
@@ -12889,12 +12889,12 @@
       </c>
       <c r="P145" t="inlineStr">
         <is>
-          <t>Replacement,Filter,TYPE,L2</t>
+          <t>Replacement Filter TYPE L2</t>
         </is>
       </c>
       <c r="Q145" t="inlineStr">
         <is>
-          <t>Replacement,Filter,TYPE,L2</t>
+          <t>Replacement Filter TYPE L2</t>
         </is>
       </c>
       <c r="R145" t="inlineStr">
@@ -12964,12 +12964,12 @@
       </c>
       <c r="P146" t="inlineStr">
         <is>
-          <t>BMW,E46,M3,Panel,Filter,Pair</t>
+          <t>BMW E46 M3 Panel Filter Pair</t>
         </is>
       </c>
       <c r="Q146" t="inlineStr">
         <is>
-          <t>BMW,E46,M3,Panel,Filter,Pair</t>
+          <t>BMW E46 M3 Panel Filter Pair</t>
         </is>
       </c>
       <c r="R146" t="inlineStr">
@@ -13041,12 +13041,12 @@
       </c>
       <c r="P147" t="inlineStr">
         <is>
-          <t>BMW,F8X,M3/M4,Panel,Filter,Pair</t>
+          <t>BMW F8X M3/M4 Panel Filter Pair</t>
         </is>
       </c>
       <c r="Q147" t="inlineStr">
         <is>
-          <t>BMW,F8X,M3/M4,Panel,Filter,Pair</t>
+          <t>BMW F8X M3/M4 Panel Filter Pair</t>
         </is>
       </c>
       <c r="R147" t="inlineStr">
@@ -13118,12 +13118,12 @@
       </c>
       <c r="P148" t="inlineStr">
         <is>
-          <t>BMW,F1X,M5/M6,Panel,Filter,Pair</t>
+          <t>BMW F1X M5/M6 Panel Filter Pair</t>
         </is>
       </c>
       <c r="Q148" t="inlineStr">
         <is>
-          <t>BMW,F1X,M5/M6,Panel,Filter,Pair</t>
+          <t>BMW F1X M5/M6 Panel Filter Pair</t>
         </is>
       </c>
       <c r="R148" t="inlineStr">
@@ -13193,12 +13193,12 @@
       </c>
       <c r="P149" t="inlineStr">
         <is>
-          <t>BMW,N55,Panel,Filter,</t>
+          <t xml:space="preserve">BMW N55 Panel Filter </t>
         </is>
       </c>
       <c r="Q149" t="inlineStr">
         <is>
-          <t>BMW,N55,Panel,Filter,</t>
+          <t xml:space="preserve">BMW N55 Panel Filter </t>
         </is>
       </c>
       <c r="R149" t="inlineStr">
@@ -13268,12 +13268,12 @@
       </c>
       <c r="P150" t="inlineStr">
         <is>
-          <t>BMW,F9X,X3M/X4M,Panel,Filter,Replacement,Set</t>
+          <t>BMW F9X X3M/X4M Panel Filter Replacement Set</t>
         </is>
       </c>
       <c r="Q150" t="inlineStr">
         <is>
-          <t>BMW,F9X,X3M/X4M,Panel,Filter,Replacement,Set</t>
+          <t>BMW F9X X3M/X4M Panel Filter Replacement Set</t>
         </is>
       </c>
       <c r="R150" t="inlineStr">
@@ -13345,12 +13345,12 @@
       </c>
       <c r="P151" t="inlineStr">
         <is>
-          <t>Panel,Filter,for,Eventuri,GLC63S,/,C63S,Intake,set,of,2</t>
+          <t>Panel Filter for Eventuri GLC63S / C63S Intake set of 2</t>
         </is>
       </c>
       <c r="Q151" t="inlineStr">
         <is>
-          <t>Panel,Filter,for,Eventuri,GLC63S,/,C63S,Intake,set,of,2</t>
+          <t>Panel Filter for Eventuri GLC63S / C63S Intake set of 2</t>
         </is>
       </c>
       <c r="R151" t="inlineStr">
@@ -13420,12 +13420,12 @@
       </c>
       <c r="P152" t="inlineStr">
         <is>
-          <t>Custom,BMC,Panel,Filter,For,C8,RS6,Intake</t>
+          <t>Custom BMC Panel Filter For C8 RS6 Intake</t>
         </is>
       </c>
       <c r="Q152" t="inlineStr">
         <is>
-          <t>Custom,BMC,Panel,Filter,For,C8,RS6,Intake</t>
+          <t>Custom BMC Panel Filter For C8 RS6 Intake</t>
         </is>
       </c>
       <c r="R152" t="inlineStr">
@@ -13492,12 +13492,12 @@
       </c>
       <c r="P153" t="inlineStr">
         <is>
-          <t>V,Badge</t>
+          <t>V Badge</t>
         </is>
       </c>
       <c r="Q153" t="inlineStr">
         <is>
-          <t>V,Badge</t>
+          <t>V Badge</t>
         </is>
       </c>
       <c r="R153" t="inlineStr">
@@ -13569,12 +13569,12 @@
       </c>
       <c r="P154" t="inlineStr">
         <is>
-          <t>Mini,Cooper,S/JCW,MAF,tube</t>
+          <t>Mini Cooper S/JCW MAF tube</t>
         </is>
       </c>
       <c r="Q154" t="inlineStr">
         <is>
-          <t>Mini,Cooper,S/JCW,MAF,tube</t>
+          <t>Mini Cooper S/JCW MAF tube</t>
         </is>
       </c>
       <c r="R154" t="inlineStr">
@@ -13646,12 +13646,12 @@
       </c>
       <c r="P155" t="inlineStr">
         <is>
-          <t>Mini,Cooper,S/JCW,Facelift,MAF,tube</t>
+          <t>Mini Cooper S/JCW Facelift MAF tube</t>
         </is>
       </c>
       <c r="Q155" t="inlineStr">
         <is>
-          <t>Mini,Cooper,S/JCW,Facelift,MAF,tube</t>
+          <t>Mini Cooper S/JCW Facelift MAF tube</t>
         </is>
       </c>
       <c r="R155" t="inlineStr">
@@ -13723,12 +13723,12 @@
       </c>
       <c r="P156" t="inlineStr">
         <is>
-          <t>Honda,FK8,Silicon,between,Intake,and,Upgraded,Chargepipe</t>
+          <t>Honda FK8 Silicon between Intake and Upgraded Chargepipe</t>
         </is>
       </c>
       <c r="Q156" t="inlineStr">
         <is>
-          <t>Honda,FK8,Silicon,between,Intake,and,Upgraded,Chargepipe</t>
+          <t>Honda FK8 Silicon between Intake and Upgraded Chargepipe</t>
         </is>
       </c>
       <c r="R156" t="inlineStr">

</xml_diff>